<commit_message>
completed overall coding for CPC152 individual assignment
</commit_message>
<xml_diff>
--- a/CPC152/assignment (individual)/notes/152 charts.xlsx
+++ b/CPC152/assignment (individual)/notes/152 charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Universiti Sains Malaysia\laptop\USM\USM coding github\CPC152\assignment (individual)\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AAFF6C-1257-4D74-95B5-5DFBFA8CF3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648B8923-9D76-4353-9B51-C0BEA2A95F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{0F0918FA-484D-4367-9B59-31E2DD79AAD2}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="10200" activeTab="2" xr2:uid="{0F0918FA-484D-4367-9B59-31E2DD79AAD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="429">
   <si>
     <t>Bar chart: You can use this to compare the counts or proportions of different categories, such as passenger class, sex, age group, survival status, etc.</t>
   </si>
@@ -1322,6 +1322,12 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -1437,7 +1443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1457,13 +1463,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1502,46 +1502,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Roboto"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Roboto"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1610,13 +1570,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -1627,6 +1580,53 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Roboto"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Roboto"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1888,18 +1888,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C05641CF-2961-4369-BBD8-FD1B34F9DC7C}" name="Table2" displayName="Table2" ref="B2:D72" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
-  <autoFilter ref="B2:D72" xr:uid="{C05641CF-2961-4369-BBD8-FD1B34F9DC7C}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="1"/>
-      </filters>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C05641CF-2961-4369-BBD8-FD1B34F9DC7C}" name="Table2" displayName="Table2" ref="B2:E72" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="B2:E72" xr:uid="{C05641CF-2961-4369-BBD8-FD1B34F9DC7C}">
+    <filterColumn colId="1">
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
-  <tableColumns count="3">
-    <tableColumn id="3" xr3:uid="{E034FDD3-CF5E-4CB7-A3E3-CB966EEBDAAE}" name="Group" dataDxfId="0"/>
-    <tableColumn id="1" xr3:uid="{81A1CC8B-31FF-4135-8171-BB3FFFCF57B1}" name="Chart" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{7E55643D-DF52-49E7-945B-2D68BF6D998C}" name="Summary" dataDxfId="3"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:E72">
+    <sortCondition ref="B2:B72"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="3" xr3:uid="{E034FDD3-CF5E-4CB7-A3E3-CB966EEBDAAE}" name="Group" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{12343150-A929-424C-A033-AE7067284D91}" name="Use"/>
+    <tableColumn id="1" xr3:uid="{81A1CC8B-31FF-4135-8171-BB3FFFCF57B1}" name="Chart" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{7E55643D-DF52-49E7-945B-2D68BF6D998C}" name="Summary" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2372,7 +2374,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="105" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" ht="90" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2401,7 +2403,7 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="2:9" ht="105" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" ht="90" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2481,7 +2483,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="2:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" ht="90" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>101</v>
       </c>
@@ -2521,7 +2523,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="2:3" ht="120" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" ht="105" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>106</v>
       </c>
@@ -2529,7 +2531,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="2:3" ht="120" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3" ht="105" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>107</v>
       </c>
@@ -2561,7 +2563,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="2:3" ht="135" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:3" ht="120" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>111</v>
       </c>
@@ -2577,7 +2579,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="120" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:3" ht="105" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>113</v>
       </c>
@@ -4278,794 +4280,839 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE66BBA-459F-4143-A5C1-97F56E7028C2}">
-  <dimension ref="B2:D72"/>
+  <dimension ref="B2:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="155" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.109375" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" customWidth="1"/>
-    <col min="3" max="3" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.5546875" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
+        <v>427</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>423</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="13" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="4" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>132</v>
+      <c r="C7" t="s">
+        <v>357</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="10" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B10">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15">
         <v>3</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="D15" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="E16" s="7" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="11" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <v>6</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B12">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B22">
         <v>4</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C22" t="s">
+        <v>357</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>357</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="E23" s="9" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="13" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B13">
-        <v>7</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B15">
-        <v>7</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B17">
-        <v>5</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B18">
-        <v>5</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B19">
-        <v>5</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B20">
-        <v>5</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B22">
-        <v>8</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B23">
-        <v>6</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>5</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" t="s">
+        <v>357</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>428</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>357</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="E29" s="9" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="25" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B25">
-        <v>8</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B26">
-        <v>8</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B27">
-        <v>8</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B28">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B30">
         <v>6</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B29">
-        <v>9</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B30">
-        <v>9</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>6</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="D31" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="E33" s="8" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="32" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B32">
-        <v>8</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B33">
-        <v>8</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>6</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" t="s">
+        <v>357</v>
+      </c>
+      <c r="D34" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="E34" s="9" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="35" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B36">
         <v>7</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C36" t="s">
+        <v>357</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>357</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="E38" s="6" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="36" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B36">
-        <v>11</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B37">
-        <v>6</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B38">
-        <v>2</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>8</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="D39" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>8</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>8</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>8</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>357</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="E45" s="10" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="40" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B40">
-        <v>11</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B41">
-        <v>11</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B42">
-        <v>11</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B43">
-        <v>3</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B44">
-        <v>2</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B45">
-        <v>3</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B46">
-        <v>2</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
+        <v>428</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B47">
-        <v>2</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="C47" t="s">
+        <v>428</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48">
-        <v>3</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>203</v>
+        <v>9</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49">
-        <v>3</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>204</v>
+        <v>9</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50">
         <v>9</v>
       </c>
-      <c r="C50" s="9" t="s">
-        <v>205</v>
-      </c>
       <c r="D50" s="9" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51">
         <v>9</v>
       </c>
-      <c r="C51" s="8" t="s">
-        <v>206</v>
-      </c>
       <c r="D51" s="8" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52">
-        <v>9</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>207</v>
+        <v>10</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53">
-        <v>9</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>208</v>
+        <v>10</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54">
         <v>10</v>
       </c>
-      <c r="C54" s="9" t="s">
-        <v>209</v>
-      </c>
       <c r="D54" s="9" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B55">
         <v>10</v>
       </c>
-      <c r="C55" s="8" t="s">
-        <v>210</v>
-      </c>
       <c r="D55" s="8" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B56">
         <v>10</v>
       </c>
-      <c r="C56" s="9" t="s">
-        <v>211</v>
-      </c>
       <c r="D56" s="9" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B57">
         <v>10</v>
       </c>
-      <c r="C57" s="8" t="s">
-        <v>212</v>
-      </c>
       <c r="D57" s="8" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58">
         <v>10</v>
       </c>
-      <c r="C58" s="9" t="s">
-        <v>213</v>
-      </c>
       <c r="D58" s="9" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B59">
-        <v>10</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B60">
-        <v>10</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>215</v>
+        <v>11</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B61">
-        <v>1</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>216</v>
+        <v>11</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B62">
         <v>11</v>
       </c>
-      <c r="C62" s="9" t="s">
-        <v>217</v>
-      </c>
       <c r="D62" s="9" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="B63">
         <v>11</v>
       </c>
-      <c r="C63" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
+        <v>357</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B64">
         <v>11</v>
       </c>
-      <c r="C64" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D64" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B65">
         <v>11</v>
       </c>
-      <c r="C65" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D65" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B66">
         <v>11</v>
       </c>
-      <c r="C66" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D66" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67">
         <v>11</v>
       </c>
-      <c r="C67" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="68" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D67" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B68">
         <v>11</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="D68" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>11</v>
+      </c>
+      <c r="D69" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="D68" s="9" t="s">
+      <c r="E69" s="9" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B69">
-        <v>1</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B70">
         <v>11</v>
       </c>
-      <c r="C70" s="9" t="s">
+      <c r="D70" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="D70" s="9" t="s">
+      <c r="E70" s="9" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="71" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B71" s="8"/>
-      <c r="C71" s="8" t="s">
+      <c r="C71" s="8"/>
+      <c r="D71" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="E71" s="8" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="72" spans="2:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="16"/>
-      <c r="C72" s="16" t="s">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B72" s="14"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="D72" s="16" t="s">
+      <c r="E72" s="14" t="s">
         <v>422</v>
       </c>
     </row>

</xml_diff>